<commit_message>
Update pay period 27 data with latest extraction (v4)
- Added Pauline Nguyen hours (86.92) - previously missing
- Increased total entries from 137 to 179 records
- Improved compliance rate to 50% (5 of 10 users)
- Updated expense totals to reflect complete data
</commit_message>
<xml_diff>
--- a/kimai-data/27/pay-period-27.xlsx
+++ b/kimai-data/27/pay-period-27.xlsx
@@ -607,13 +607,13 @@
         <f>F11 + G11</f>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I11" t="str">
-        <v>Short 80.00 hours</v>
+        <v>Extra 6.92 hours carry over</v>
       </c>
     </row>
     <row r="12">

</xml_diff>